<commit_message>
summary:     Test updates. date:        Wed Aug 25 12:21:58 2010 +0000 user:        paulbartrum changeset:   144:a67d810753df hg2git:      Preserving hg log changeset
</commit_message>
<xml_diff>
--- a/Sputnik/Results.xlsx
+++ b/Sputnik/Results.xlsx
@@ -110,7 +110,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38819444444444451"/>
+          <c:x val="0.38819444444444456"/>
           <c:y val="2.3148148148148147E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -140,6 +140,10 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:spPr/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
             <c:spPr>
               <a:gradFill>
                 <a:gsLst>
@@ -155,9 +159,9 @@
                     </a:srgbClr>
                   </a:gs>
                   <a:gs pos="61000">
-                    <a:schemeClr val="accent3">
+                    <a:srgbClr val="9BBB59">
                       <a:lumMod val="75000"/>
-                    </a:schemeClr>
+                    </a:srgbClr>
                   </a:gs>
                 </a:gsLst>
                 <a:lin ang="5400000" scaled="0"/>
@@ -173,10 +177,10 @@
                   <c:v>Internet Explorer 8</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Firefox 3.6.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Jurassic</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Firefox 3.6.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Chrome 5</c:v>
@@ -194,10 +198,10 @@
                   <c:v>463</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>388</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>264</c:v>
+                  <c:v>253</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>227</c:v>
@@ -206,24 +210,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="78192000"/>
-        <c:axId val="105448576"/>
+        <c:axId val="72683520"/>
+        <c:axId val="72685056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78192000"/>
+        <c:axId val="72683520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105448576"/>
+        <c:crossAx val="72685056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105448576"/>
+        <c:axId val="72685056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -231,7 +235,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78192000"/>
+        <c:crossAx val="72683520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -240,7 +244,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -569,7 +573,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -596,18 +600,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>388</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:2">

</xml_diff>

<commit_message>
summary:     Updated sputnik results. date:        Tue Aug 31 07:28:30 2010 +0000 user:        paulbartrum changeset:   158:1614573c2949 hg2git:      Preserving hg log changeset
</commit_message>
<xml_diff>
--- a/Sputnik/Results.xlsx
+++ b/Sputnik/Results.xlsx
@@ -110,7 +110,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38819444444444456"/>
+          <c:x val="0.38819444444444462"/>
           <c:y val="2.3148148148148147E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -144,6 +144,10 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:spPr/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
             <c:spPr>
               <a:gradFill>
                 <a:gsLst>
@@ -180,10 +184,10 @@
                   <c:v>Firefox 3.6.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Chrome 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Jurassic</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Chrome 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -201,33 +205,33 @@
                   <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>253</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>227</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="72683520"/>
-        <c:axId val="72685056"/>
+        <c:axId val="71827840"/>
+        <c:axId val="71829376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="72683520"/>
+        <c:axId val="71827840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72685056"/>
+        <c:crossAx val="71829376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72685056"/>
+        <c:axId val="71829376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -235,7 +239,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72683520"/>
+        <c:crossAx val="71827840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -244,7 +248,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -573,7 +577,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -608,18 +612,18 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>253</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>227</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
summary:     Updated results. date:        Tue Sep 07 00:45:59 2010 +0000 user:        paulbartrum changeset:   166:1efd1949e118 hg2git:      Preserving hg log changeset
</commit_message>
<xml_diff>
--- a/Sputnik/Results.xlsx
+++ b/Sputnik/Results.xlsx
@@ -110,7 +110,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38819444444444462"/>
+          <c:x val="0.38819444444444468"/>
           <c:y val="2.3148148148148147E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -136,15 +136,12 @@
           </c:tx>
           <c:dPt>
             <c:idx val="0"/>
-            <c:spPr/>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:spPr/>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:spPr/>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -208,30 +205,30 @@
                   <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>202</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="71827840"/>
-        <c:axId val="71829376"/>
+        <c:axId val="81269504"/>
+        <c:axId val="81271040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71827840"/>
+        <c:axId val="81269504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71829376"/>
+        <c:crossAx val="81271040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71829376"/>
+        <c:axId val="81271040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -239,7 +236,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71827840"/>
+        <c:crossAx val="81269504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -248,7 +245,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -577,7 +574,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -623,7 +620,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>202</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
summary:     Updated sputnik results. date:        Wed Sep 08 14:23:46 2010 +0000 user:        paulbartrum changeset:   181:ca50ed3ccf37 hg2git:      Preserving hg log changeset
</commit_message>
<xml_diff>
--- a/Sputnik/Results.xlsx
+++ b/Sputnik/Results.xlsx
@@ -104,13 +104,27 @@
               <a:t>Sputnik v2</a:t>
             </a:r>
           </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>(shorter bars</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> are better)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
         </c:rich>
       </c:tx>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38819444444444468"/>
+          <c:x val="0.38819444444444484"/>
           <c:y val="2.3148148148148147E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -134,15 +148,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:dPt>
-            <c:idx val="0"/>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-          </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
             <c:spPr>
@@ -205,38 +210,63 @@
                   <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="81269504"/>
-        <c:axId val="81271040"/>
+        <c:axId val="83504512"/>
+        <c:axId val="108405888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81269504"/>
+        <c:axId val="83504512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81271040"/>
+        <c:crossAx val="108405888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81271040"/>
+        <c:axId val="108405888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number of failures</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.492682678734577"/>
+              <c:y val="0.88726164548580366"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81269504"/>
+        <c:crossAx val="83504512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -245,7 +275,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -258,13 +288,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>28576</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -574,7 +604,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>